<commit_message>
round 7 and 8 updates and predictions.
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Carlton_stats.xlsx
+++ b/AFL_ML/Data/Carlton_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JU102"/>
+  <dimension ref="A1:JV102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GS74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="GV98" activeCellId="0" sqref="GV98"/>
@@ -1299,8 +1299,11 @@
       <c r="JT1" s="1" t="n">
         <v>10801</v>
       </c>
-      <c r="JU1" t="n">
+      <c r="JU1" s="1" t="n">
         <v>10801</v>
+      </c>
+      <c r="JV1" t="n">
+        <v>10810</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -2146,7 +2149,10 @@
       <c r="JT2" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="JU2" t="n">
+      <c r="JU2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JV2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -2993,8 +2999,11 @@
       <c r="JT3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JU3" t="n">
+      <c r="JU3" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JV3" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3840,8 +3849,11 @@
       <c r="JT4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JU4" t="n">
+      <c r="JU4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JV4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4687,7 +4699,10 @@
       <c r="JT5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JU5" t="n">
+      <c r="JU5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JV5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5534,8 +5549,11 @@
       <c r="JT6" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="JU6" t="n">
+      <c r="JU6" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="JV6" t="n">
+        <v>152</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -6381,8 +6399,11 @@
       <c r="JT7" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="JU7" t="n">
+      <c r="JU7" s="1" t="n">
         <v>82</v>
+      </c>
+      <c r="JV7" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -7228,8 +7249,11 @@
       <c r="JT8" s="1" t="n">
         <v>-22</v>
       </c>
-      <c r="JU8" t="n">
+      <c r="JU8" s="1" t="n">
         <v>-22</v>
+      </c>
+      <c r="JV8" t="n">
+        <v>108</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -8075,8 +8099,11 @@
       <c r="JT9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JU9" t="n">
+      <c r="JU9" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JV9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -8922,8 +8949,11 @@
       <c r="JT10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JU10" t="n">
+      <c r="JU10" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="JV10" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -9769,8 +9799,11 @@
       <c r="JT11" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="JU11" t="n">
+      <c r="JU11" s="1" t="n">
         <v>256</v>
+      </c>
+      <c r="JV11" t="n">
+        <v>261</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -10616,8 +10649,11 @@
       <c r="JT12" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="JU12" t="n">
+      <c r="JU12" s="1" t="n">
         <v>190</v>
+      </c>
+      <c r="JV12" t="n">
+        <v>191</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -11463,8 +11499,11 @@
       <c r="JT13" s="1" t="n">
         <v>446</v>
       </c>
-      <c r="JU13" t="n">
+      <c r="JU13" s="1" t="n">
         <v>446</v>
+      </c>
+      <c r="JV13" t="n">
+        <v>452</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -12310,8 +12349,11 @@
       <c r="JT14" s="1" t="n">
         <v>1.35</v>
       </c>
-      <c r="JU14" t="n">
+      <c r="JU14" s="1" t="n">
         <v>1.35</v>
+      </c>
+      <c r="JV14" t="n">
+        <v>1.37</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -13157,8 +13199,11 @@
       <c r="JT15" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="JU15" t="n">
+      <c r="JU15" s="1" t="n">
         <v>140</v>
+      </c>
+      <c r="JV15" t="n">
+        <v>137</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -14004,8 +14049,11 @@
       <c r="JT16" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="JU16" t="n">
+      <c r="JU16" s="1" t="n">
         <v>47</v>
+      </c>
+      <c r="JV16" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -14851,8 +14899,11 @@
       <c r="JT17" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JU17" t="n">
+      <c r="JU17" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="JV17" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -15698,8 +15749,11 @@
       <c r="JT18" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JU18" t="n">
+      <c r="JU18" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="JV18" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -16545,8 +16599,11 @@
       <c r="JT19" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="JU19" t="n">
+      <c r="JU19" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="JV19" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -17392,8 +17449,11 @@
       <c r="JT20" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JU20" t="n">
+      <c r="JU20" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JV20" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -18239,8 +18299,11 @@
       <c r="JT21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JU21" t="n">
+      <c r="JU21" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JV21" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -19086,8 +19149,11 @@
       <c r="JT22" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="JU22" t="n">
+      <c r="JU22" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="JV22" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -19933,8 +19999,11 @@
       <c r="JT23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JU23" t="n">
+      <c r="JU23" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="JV23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -20780,8 +20849,11 @@
       <c r="JT24" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JU24" t="n">
+      <c r="JU24" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="JV24" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -21627,8 +21699,11 @@
       <c r="JT25" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JU25" t="n">
+      <c r="JU25" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JV25" t="n">
+        <v>62.2</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -22474,8 +22549,11 @@
       <c r="JT26" s="1" t="n">
         <v>55.75</v>
       </c>
-      <c r="JU26" t="n">
+      <c r="JU26" s="1" t="n">
         <v>55.75</v>
+      </c>
+      <c r="JV26" t="n">
+        <v>19.65</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -23321,8 +23399,11 @@
       <c r="JT27" s="1" t="n">
         <v>22.3</v>
       </c>
-      <c r="JU27" t="n">
+      <c r="JU27" s="1" t="n">
         <v>22.3</v>
+      </c>
+      <c r="JV27" t="n">
+        <v>12.22</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -24168,8 +24249,11 @@
       <c r="JT28" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="JU28" t="n">
+      <c r="JU28" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="JV28" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -25015,8 +25099,11 @@
       <c r="JT29" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JU29" t="n">
+      <c r="JU29" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="JV29" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -25862,8 +25949,11 @@
       <c r="JT30" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="JU30" t="n">
+      <c r="JU30" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="JV30" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -26709,8 +26799,11 @@
       <c r="JT31" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JU31" t="n">
+      <c r="JU31" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="JV31" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -27556,8 +27649,11 @@
       <c r="JT32" s="1" t="n">
         <v>2.6</v>
       </c>
-      <c r="JU32" t="n">
+      <c r="JU32" s="1" t="n">
         <v>2.6</v>
+      </c>
+      <c r="JV32" t="n">
+        <v>1.51</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -28403,8 +28499,11 @@
       <c r="JT33" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="JU33" t="n">
+      <c r="JU33" s="1" t="n">
         <v>6.5</v>
+      </c>
+      <c r="JV33" t="n">
+        <v>2.43</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -29250,8 +29349,11 @@
       <c r="JT34" s="1" t="n">
         <v>36.5</v>
       </c>
-      <c r="JU34" t="n">
+      <c r="JU34" s="1" t="n">
         <v>36.5</v>
+      </c>
+      <c r="JV34" t="n">
+        <v>62.5</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -30097,8 +30199,11 @@
       <c r="JT35" s="1" t="n">
         <v>15.4</v>
       </c>
-      <c r="JU35" t="n">
+      <c r="JU35" s="1" t="n">
         <v>15.4</v>
+      </c>
+      <c r="JV35" t="n">
+        <v>41.1</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -30944,8 +31049,11 @@
       <c r="JT36" s="1" t="n">
         <v>188.4</v>
       </c>
-      <c r="JU36" t="n">
+      <c r="JU36" s="1" t="n">
         <v>188.4</v>
+      </c>
+      <c r="JV36" t="n">
+        <v>188.7</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -31791,8 +31899,11 @@
       <c r="JT37" s="1" t="n">
         <v>87.5</v>
       </c>
-      <c r="JU37" t="n">
+      <c r="JU37" s="1" t="n">
         <v>87.5</v>
+      </c>
+      <c r="JV37" t="n">
+        <v>87.90000000000001</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -32638,8 +32749,11 @@
       <c r="JT38" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="JU38" t="n">
+      <c r="JU38" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="JV38" t="n">
+        <v>25.8</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -33485,8 +33599,11 @@
       <c r="JT39" s="1" t="n">
         <v>80.40000000000001</v>
       </c>
-      <c r="JU39" t="n">
+      <c r="JU39" s="1" t="n">
         <v>80.40000000000001</v>
+      </c>
+      <c r="JV39" t="n">
+        <v>91.09999999999999</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -34332,8 +34449,11 @@
       <c r="JT40" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JU40" t="n">
+      <c r="JU40" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JV40" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -35179,7 +35299,10 @@
       <c r="JT41" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JU41" t="n">
+      <c r="JU41" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JV41" t="n">
         <v>7</v>
       </c>
     </row>
@@ -36026,8 +36149,11 @@
       <c r="JT42" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JU42" t="n">
+      <c r="JU42" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JV42" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="43" ht="13.8" customHeight="1" s="2">
@@ -36873,8 +36999,11 @@
       <c r="JT43" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JU43" t="n">
+      <c r="JU43" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JV43" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -37720,8 +37849,11 @@
       <c r="JT44" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="JU44" t="n">
+      <c r="JU44" s="1" t="n">
         <v>140</v>
+      </c>
+      <c r="JV44" t="n">
+        <v>138</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -38567,8 +38699,11 @@
       <c r="JT45" s="1" t="n">
         <v>304</v>
       </c>
-      <c r="JU45" t="n">
+      <c r="JU45" s="1" t="n">
         <v>304</v>
+      </c>
+      <c r="JV45" t="n">
+        <v>307</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -39414,8 +39549,11 @@
       <c r="JT46" s="1" t="n">
         <v>341</v>
       </c>
-      <c r="JU46" t="n">
+      <c r="JU46" s="1" t="n">
         <v>341</v>
+      </c>
+      <c r="JV46" t="n">
+        <v>354</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -40261,8 +40399,11 @@
       <c r="JT47" s="1" t="n">
         <v>76.5</v>
       </c>
-      <c r="JU47" t="n">
+      <c r="JU47" s="1" t="n">
         <v>76.5</v>
+      </c>
+      <c r="JV47" t="n">
+        <v>78.3</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -41108,8 +41249,11 @@
       <c r="JT48" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JU48" t="n">
+      <c r="JU48" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="JV48" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -41955,7 +42099,10 @@
       <c r="JT49" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="JU49" t="n">
+      <c r="JU49" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JV49" t="n">
         <v>14</v>
       </c>
     </row>
@@ -42802,8 +42949,11 @@
       <c r="JT50" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JU50" t="n">
+      <c r="JU50" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JV50" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -43649,8 +43799,11 @@
       <c r="JT51" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="JU51" t="n">
+      <c r="JU51" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="JV51" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -44496,8 +44649,11 @@
       <c r="JT52" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="JU52" t="n">
+      <c r="JU52" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="JV52" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -45343,7 +45499,10 @@
       <c r="JT53" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="JU53" t="n">
+      <c r="JU53" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="JV53" t="n">
         <v>46</v>
       </c>
     </row>
@@ -46190,8 +46349,11 @@
       <c r="JT54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JU54" t="n">
+      <c r="JU54" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JV54" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -47037,8 +47199,11 @@
       <c r="JT55" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JU55" t="n">
+      <c r="JU55" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JV55" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -47884,8 +48049,11 @@
       <c r="JT56" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="JU56" t="n">
+      <c r="JU56" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="JV56" t="n">
+        <v>82.59999999999999</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -48731,8 +48899,11 @@
       <c r="JT57" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="JU57" t="n">
+      <c r="JU57" s="1" t="n">
         <v>220</v>
+      </c>
+      <c r="JV57" t="n">
+        <v>156</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -49578,8 +49749,11 @@
       <c r="JT58" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="JU58" t="n">
+      <c r="JU58" s="1" t="n">
         <v>140</v>
+      </c>
+      <c r="JV58" t="n">
+        <v>129</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -50425,8 +50599,11 @@
       <c r="JT59" s="1" t="n">
         <v>360</v>
       </c>
-      <c r="JU59" t="n">
+      <c r="JU59" s="1" t="n">
         <v>360</v>
+      </c>
+      <c r="JV59" t="n">
+        <v>285</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -51272,8 +51449,11 @@
       <c r="JT60" s="1" t="n">
         <v>1.57</v>
       </c>
-      <c r="JU60" t="n">
+      <c r="JU60" s="1" t="n">
         <v>1.57</v>
+      </c>
+      <c r="JV60" t="n">
+        <v>1.21</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -52119,8 +52299,11 @@
       <c r="JT61" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="JU61" t="n">
+      <c r="JU61" s="1" t="n">
         <v>101</v>
+      </c>
+      <c r="JV61" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -52966,8 +53149,11 @@
       <c r="JT62" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="JU62" t="n">
+      <c r="JU62" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="JV62" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -53813,8 +53999,11 @@
       <c r="JT63" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="JU63" t="n">
+      <c r="JU63" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="JV63" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -54660,8 +54849,11 @@
       <c r="JT64" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="JU64" t="n">
+      <c r="JU64" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="JV64" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -55507,8 +55699,11 @@
       <c r="JT65" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JU65" t="n">
+      <c r="JU65" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="JV65" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -56354,8 +56549,11 @@
       <c r="JT66" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JU66" t="n">
+      <c r="JU66" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JV66" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -57201,8 +57399,11 @@
       <c r="JT67" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JU67" t="n">
+      <c r="JU67" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JV67" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -58048,8 +58249,11 @@
       <c r="JT68" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JU68" t="n">
+      <c r="JU68" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JV68" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -58895,8 +59099,11 @@
       <c r="JT69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JU69" t="n">
+      <c r="JU69" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JV69" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -59742,8 +59949,11 @@
       <c r="JT70" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="JU70" t="n">
+      <c r="JU70" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="JV70" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -60589,8 +60799,11 @@
       <c r="JT71" s="1" t="n">
         <v>54.5</v>
       </c>
-      <c r="JU71" t="n">
+      <c r="JU71" s="1" t="n">
         <v>54.5</v>
+      </c>
+      <c r="JV71" t="n">
+        <v>42.9</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -61436,8 +61649,11 @@
       <c r="JT72" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="JU72" t="n">
+      <c r="JU72" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="JV72" t="n">
+        <v>47.5</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -62283,8 +62499,11 @@
       <c r="JT73" s="1" t="n">
         <v>16.36</v>
       </c>
-      <c r="JU73" t="n">
+      <c r="JU73" s="1" t="n">
         <v>16.36</v>
+      </c>
+      <c r="JV73" t="n">
+        <v>20.36</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -63130,8 +63349,11 @@
       <c r="JT74" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="JU74" t="n">
+      <c r="JU74" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="JV74" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -63977,8 +64199,11 @@
       <c r="JT75" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JU75" t="n">
+      <c r="JU75" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="JV75" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -64824,8 +65049,11 @@
       <c r="JT76" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="JU76" t="n">
+      <c r="JU76" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="JV76" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -65671,8 +65899,11 @@
       <c r="JT77" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="JU77" t="n">
+      <c r="JU77" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="JV77" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -66518,8 +66749,11 @@
       <c r="JT78" s="1" t="n">
         <v>2.55</v>
       </c>
-      <c r="JU78" t="n">
+      <c r="JU78" s="1" t="n">
         <v>2.55</v>
+      </c>
+      <c r="JV78" t="n">
+        <v>2.43</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -67365,8 +67599,11 @@
       <c r="JT79" s="1" t="n">
         <v>4.67</v>
       </c>
-      <c r="JU79" t="n">
+      <c r="JU79" s="1" t="n">
         <v>4.67</v>
+      </c>
+      <c r="JV79" t="n">
+        <v>5.67</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -68212,8 +68449,11 @@
       <c r="JT80" s="1" t="n">
         <v>33.9</v>
       </c>
-      <c r="JU80" t="n">
+      <c r="JU80" s="1" t="n">
         <v>33.9</v>
+      </c>
+      <c r="JV80" t="n">
+        <v>35.3</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -69059,8 +69299,11 @@
       <c r="JT81" s="1" t="n">
         <v>21.4</v>
       </c>
-      <c r="JU81" t="n">
+      <c r="JU81" s="1" t="n">
         <v>21.4</v>
+      </c>
+      <c r="JV81" t="n">
+        <v>17.6</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -69906,8 +70149,11 @@
       <c r="JT82" s="1" t="n">
         <v>187.3</v>
       </c>
-      <c r="JU82" t="n">
+      <c r="JU82" s="1" t="n">
         <v>187.3</v>
+      </c>
+      <c r="JV82" t="n">
+        <v>189.2</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -70753,8 +70999,11 @@
       <c r="JT83" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="JU83" t="n">
+      <c r="JU83" s="1" t="n">
         <v>86</v>
+      </c>
+      <c r="JV83" t="n">
+        <v>87.5</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -71600,8 +71849,11 @@
       <c r="JT84" s="1" t="n">
         <v>25.41</v>
       </c>
-      <c r="JU84" t="n">
+      <c r="JU84" s="1" t="n">
         <v>25.41</v>
+      </c>
+      <c r="JV84" t="n">
+        <v>25.16</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -72447,8 +72699,11 @@
       <c r="JT85" s="1" t="n">
         <v>94.2</v>
       </c>
-      <c r="JU85" t="n">
+      <c r="JU85" s="1" t="n">
         <v>94.2</v>
+      </c>
+      <c r="JV85" t="n">
+        <v>87.40000000000001</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -73294,8 +73549,11 @@
       <c r="JT86" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JU86" t="n">
+      <c r="JU86" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JV86" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -74141,8 +74399,11 @@
       <c r="JT87" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JU87" t="n">
+      <c r="JU87" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JV87" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -74988,8 +75249,11 @@
       <c r="JT88" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JU88" t="n">
+      <c r="JU88" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JV88" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -75835,7 +76099,10 @@
       <c r="JT89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JU89" t="n">
+      <c r="JU89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JV89" t="n">
         <v>3</v>
       </c>
     </row>
@@ -76682,8 +76949,11 @@
       <c r="JT90" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="JU90" t="n">
+      <c r="JU90" s="1" t="n">
         <v>120</v>
+      </c>
+      <c r="JV90" t="n">
+        <v>115</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -77529,8 +77799,11 @@
       <c r="JT91" s="1" t="n">
         <v>231</v>
       </c>
-      <c r="JU91" t="n">
+      <c r="JU91" s="1" t="n">
         <v>231</v>
+      </c>
+      <c r="JV91" t="n">
+        <v>159</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -78376,8 +78649,11 @@
       <c r="JT92" s="1" t="n">
         <v>264</v>
       </c>
-      <c r="JU92" t="n">
+      <c r="JU92" s="1" t="n">
         <v>264</v>
+      </c>
+      <c r="JV92" t="n">
+        <v>189</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -79223,8 +79499,11 @@
       <c r="JT93" s="1" t="n">
         <v>73.3</v>
       </c>
-      <c r="JU93" t="n">
+      <c r="JU93" s="1" t="n">
         <v>73.3</v>
+      </c>
+      <c r="JV93" t="n">
+        <v>66.3</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -80070,8 +80349,11 @@
       <c r="JT94" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JU94" t="n">
+      <c r="JU94" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="JV94" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -80917,8 +81199,11 @@
       <c r="JT95" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JU95" t="n">
+      <c r="JU95" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JV95" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -81764,8 +82049,11 @@
       <c r="JT96" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JU96" t="n">
+      <c r="JU96" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JV96" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -82611,8 +82899,11 @@
       <c r="JT97" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="JU97" t="n">
+      <c r="JU97" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="JV97" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -83458,8 +83749,11 @@
       <c r="JT98" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="JU98" t="n">
+      <c r="JU98" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="JV98" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -84305,8 +84599,11 @@
       <c r="JT99" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="JU99" t="n">
+      <c r="JU99" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="JV99" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -85152,8 +85449,11 @@
       <c r="JT100" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JU100" t="n">
+      <c r="JU100" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JV100" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -85999,8 +86299,11 @@
       <c r="JT101" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JU101" t="n">
+      <c r="JU101" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JV101" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -86846,8 +87149,11 @@
       <c r="JT102" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="JU102" t="n">
+      <c r="JU102" s="1" t="n">
         <v>66.7</v>
+      </c>
+      <c r="JV102" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 4 update and round 5 predict
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Carlton_stats.xlsx
+++ b/AFL_ML/Data/Carlton_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:KU102"/>
+  <dimension ref="A1:KW102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="JR89" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="JY93" activeCellId="0" sqref="JY93"/>
@@ -1381,8 +1381,14 @@
       <c r="KT1" s="2" t="n">
         <v>11175</v>
       </c>
-      <c r="KU1" t="n">
+      <c r="KU1" s="2" t="n">
         <v>10971</v>
+      </c>
+      <c r="KV1" s="2" t="n">
+        <v>10989</v>
+      </c>
+      <c r="KW1" t="n">
+        <v>11000</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="3">
@@ -2306,7 +2312,13 @@
       <c r="KT2" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="KU2" t="n">
+      <c r="KU2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KV2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KW2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -3231,8 +3243,14 @@
       <c r="KT3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KU3" t="n">
+      <c r="KU3" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="KV3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="KW3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="3">
@@ -4156,8 +4174,14 @@
       <c r="KT4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KU4" t="n">
+      <c r="KU4" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="KV4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KW4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="3">
@@ -5081,8 +5105,14 @@
       <c r="KT5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KU5" t="n">
+      <c r="KU5" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="KV5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KW5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="3">
@@ -6006,8 +6036,14 @@
       <c r="KT6" s="2" t="n">
         <v>86</v>
       </c>
-      <c r="KU6" t="n">
+      <c r="KU6" s="2" t="n">
         <v>86</v>
+      </c>
+      <c r="KV6" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="KW6" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="3">
@@ -6931,8 +6967,14 @@
       <c r="KT7" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="KU7" t="n">
+      <c r="KU7" s="2" t="n">
         <v>81</v>
+      </c>
+      <c r="KV7" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="KW7" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="3">
@@ -7856,8 +7898,14 @@
       <c r="KT8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KU8" t="n">
+      <c r="KU8" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="KV8" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="KW8" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="3">
@@ -8781,7 +8829,13 @@
       <c r="KT9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KU9" t="n">
+      <c r="KU9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KV9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KW9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9706,8 +9760,14 @@
       <c r="KT10" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KU10" t="n">
+      <c r="KU10" s="2" t="n">
         <v>14</v>
+      </c>
+      <c r="KV10" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="KW10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="3">
@@ -10631,8 +10691,14 @@
       <c r="KT11" s="2" t="n">
         <v>216</v>
       </c>
-      <c r="KU11" t="n">
+      <c r="KU11" s="2" t="n">
         <v>218</v>
+      </c>
+      <c r="KV11" s="2" t="n">
+        <v>225</v>
+      </c>
+      <c r="KW11" t="n">
+        <v>219</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="3">
@@ -11556,8 +11622,14 @@
       <c r="KT12" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="KU12" t="n">
+      <c r="KU12" s="2" t="n">
         <v>137</v>
+      </c>
+      <c r="KV12" s="2" t="n">
+        <v>141</v>
+      </c>
+      <c r="KW12" t="n">
+        <v>134</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="3">
@@ -12481,8 +12553,14 @@
       <c r="KT13" s="2" t="n">
         <v>341</v>
       </c>
-      <c r="KU13" t="n">
+      <c r="KU13" s="2" t="n">
         <v>355</v>
+      </c>
+      <c r="KV13" s="2" t="n">
+        <v>366</v>
+      </c>
+      <c r="KW13" t="n">
+        <v>353</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="3">
@@ -13406,8 +13484,14 @@
       <c r="KT14" s="2" t="n">
         <v>1.73</v>
       </c>
-      <c r="KU14" t="n">
+      <c r="KU14" s="2" t="n">
         <v>1.59</v>
+      </c>
+      <c r="KV14" s="2" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="KW14" t="n">
+        <v>1.63</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="3">
@@ -14331,8 +14415,14 @@
       <c r="KT15" s="2" t="n">
         <v>91</v>
       </c>
-      <c r="KU15" t="n">
+      <c r="KU15" s="2" t="n">
         <v>98</v>
+      </c>
+      <c r="KV15" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="KW15" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="3">
@@ -15256,8 +15346,14 @@
       <c r="KT16" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="KU16" t="n">
+      <c r="KU16" s="2" t="n">
         <v>69</v>
+      </c>
+      <c r="KV16" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="KW16" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="3">
@@ -16181,8 +16277,14 @@
       <c r="KT17" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="KU17" t="n">
+      <c r="KU17" s="2" t="n">
         <v>31</v>
+      </c>
+      <c r="KV17" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="KW17" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="3">
@@ -17106,8 +17208,14 @@
       <c r="KT18" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="KU18" t="n">
+      <c r="KU18" s="2" t="n">
         <v>24</v>
+      </c>
+      <c r="KV18" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="KW18" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="3">
@@ -18031,8 +18139,14 @@
       <c r="KT19" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="KU19" t="n">
+      <c r="KU19" s="2" t="n">
         <v>17</v>
+      </c>
+      <c r="KV19" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="KW19" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="3">
@@ -18956,8 +19070,14 @@
       <c r="KT20" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KU20" t="n">
+      <c r="KU20" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="KV20" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="KW20" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="3">
@@ -19881,8 +20001,14 @@
       <c r="KT21" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KU21" t="n">
+      <c r="KU21" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="KV21" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="KW21" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="3">
@@ -20806,7 +20932,13 @@
       <c r="KT22" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="KU22" t="n">
+      <c r="KU22" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="KV22" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KW22" t="n">
         <v>12</v>
       </c>
     </row>
@@ -21731,8 +21863,14 @@
       <c r="KT23" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="KU23" t="n">
+      <c r="KU23" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="KV23" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KW23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="3">
@@ -22656,8 +22794,14 @@
       <c r="KT24" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="KU24" t="n">
+      <c r="KU24" s="2" t="n">
         <v>26</v>
+      </c>
+      <c r="KV24" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="KW24" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="3">
@@ -23581,8 +23725,14 @@
       <c r="KT25" s="2" t="n">
         <v>61.9</v>
       </c>
-      <c r="KU25" t="n">
+      <c r="KU25" s="2" t="n">
         <v>46.2</v>
+      </c>
+      <c r="KV25" s="2" t="n">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="KW25" t="n">
+        <v>43.5</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="3">
@@ -24506,8 +24656,14 @@
       <c r="KT26" s="2" t="n">
         <v>26.23</v>
       </c>
-      <c r="KU26" t="n">
+      <c r="KU26" s="2" t="n">
         <v>29.58</v>
+      </c>
+      <c r="KV26" s="2" t="n">
+        <v>17.43</v>
+      </c>
+      <c r="KW26" t="n">
+        <v>35.3</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="3">
@@ -25431,8 +25587,14 @@
       <c r="KT27" s="2" t="n">
         <v>16.24</v>
       </c>
-      <c r="KU27" t="n">
+      <c r="KU27" s="2" t="n">
         <v>13.65</v>
+      </c>
+      <c r="KV27" s="2" t="n">
+        <v>11.44</v>
+      </c>
+      <c r="KW27" t="n">
+        <v>15.35</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="3">
@@ -26356,8 +26518,14 @@
       <c r="KT28" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="KU28" t="n">
+      <c r="KU28" s="2" t="n">
         <v>29</v>
+      </c>
+      <c r="KV28" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KW28" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="3">
@@ -27281,8 +27449,14 @@
       <c r="KT29" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="KU29" t="n">
+      <c r="KU29" s="2" t="n">
         <v>52</v>
+      </c>
+      <c r="KV29" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KW29" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="3">
@@ -28206,8 +28380,14 @@
       <c r="KT30" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KU30" t="n">
+      <c r="KU30" s="2" t="n">
         <v>37</v>
+      </c>
+      <c r="KV30" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KW30" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="3">
@@ -29131,8 +29311,14 @@
       <c r="KT31" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="KU31" t="n">
+      <c r="KU31" s="2" t="n">
         <v>65</v>
+      </c>
+      <c r="KV31" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="KW31" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="3">
@@ -30056,8 +30242,14 @@
       <c r="KT32" s="2" t="n">
         <v>2.33</v>
       </c>
-      <c r="KU32" t="n">
+      <c r="KU32" s="2" t="n">
         <v>2.5</v>
+      </c>
+      <c r="KV32" s="2" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="KW32" t="n">
+        <v>2.09</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="3">
@@ -30981,8 +31173,14 @@
       <c r="KT33" s="2" t="n">
         <v>3.77</v>
       </c>
-      <c r="KU33" t="n">
+      <c r="KU33" s="2" t="n">
         <v>5.42</v>
+      </c>
+      <c r="KV33" s="2" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="KW33" t="n">
+        <v>4.8</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="3">
@@ -31906,8 +32104,14 @@
       <c r="KT34" s="2" t="n">
         <v>34.7</v>
       </c>
-      <c r="KU34" t="n">
+      <c r="KU34" s="2" t="n">
         <v>36.9</v>
+      </c>
+      <c r="KV34" s="2" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="KW34" t="n">
+        <v>45.8</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="3">
@@ -32831,8 +33035,14 @@
       <c r="KT35" s="2" t="n">
         <v>26.5</v>
       </c>
-      <c r="KU35" t="n">
+      <c r="KU35" s="2" t="n">
         <v>18.5</v>
+      </c>
+      <c r="KV35" s="2" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="KW35" t="n">
+        <v>20.8</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="3">
@@ -33756,7 +33966,13 @@
       <c r="KT36" s="2" t="n">
         <v>188.1</v>
       </c>
-      <c r="KU36" t="n">
+      <c r="KU36" s="2" t="n">
+        <v>187.5</v>
+      </c>
+      <c r="KV36" s="2" t="n">
+        <v>187.5</v>
+      </c>
+      <c r="KW36" t="n">
         <v>187.5</v>
       </c>
     </row>
@@ -34681,8 +34897,14 @@
       <c r="KT37" s="2" t="n">
         <v>86.59999999999999</v>
       </c>
-      <c r="KU37" t="n">
+      <c r="KU37" s="2" t="n">
         <v>86.09999999999999</v>
+      </c>
+      <c r="KV37" s="2" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="KW37" t="n">
+        <v>86.3</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="3">
@@ -35606,8 +35828,14 @@
       <c r="KT38" s="2" t="n">
         <v>26.58</v>
       </c>
-      <c r="KU38" t="n">
+      <c r="KU38" s="2" t="n">
         <v>26.24</v>
+      </c>
+      <c r="KV38" s="2" t="n">
+        <v>26.24</v>
+      </c>
+      <c r="KW38" t="n">
+        <v>26.8</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="3">
@@ -36531,8 +36759,14 @@
       <c r="KT39" s="2" t="n">
         <v>92.5</v>
       </c>
-      <c r="KU39" t="n">
+      <c r="KU39" s="2" t="n">
         <v>87.7</v>
+      </c>
+      <c r="KV39" s="2" t="n">
+        <v>92.7</v>
+      </c>
+      <c r="KW39" t="n">
+        <v>92.09999999999999</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="3">
@@ -37456,8 +37690,14 @@
       <c r="KT40" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="KU40" t="n">
+      <c r="KU40" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="KV40" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KW40" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="3">
@@ -38381,8 +38621,14 @@
       <c r="KT41" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KU41" t="n">
+      <c r="KU41" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="KV41" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KW41" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="3">
@@ -39306,7 +39552,13 @@
       <c r="KT42" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KU42" t="n">
+      <c r="KU42" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KV42" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KW42" t="n">
         <v>8</v>
       </c>
     </row>
@@ -40231,8 +40483,14 @@
       <c r="KT43" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="KU43" t="n">
+      <c r="KU43" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="KV43" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="KW43" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="3">
@@ -41156,8 +41414,14 @@
       <c r="KT44" s="2" t="n">
         <v>141</v>
       </c>
-      <c r="KU44" t="n">
+      <c r="KU44" s="2" t="n">
         <v>131</v>
+      </c>
+      <c r="KV44" s="2" t="n">
+        <v>141</v>
+      </c>
+      <c r="KW44" t="n">
+        <v>136</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="3">
@@ -42081,8 +42345,14 @@
       <c r="KT45" s="2" t="n">
         <v>191</v>
       </c>
-      <c r="KU45" t="n">
+      <c r="KU45" s="2" t="n">
         <v>219</v>
+      </c>
+      <c r="KV45" s="2" t="n">
+        <v>224</v>
+      </c>
+      <c r="KW45" t="n">
+        <v>215</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="3">
@@ -43006,8 +43276,14 @@
       <c r="KT46" s="2" t="n">
         <v>249</v>
       </c>
-      <c r="KU46" t="n">
+      <c r="KU46" s="2" t="n">
         <v>257</v>
+      </c>
+      <c r="KV46" s="2" t="n">
+        <v>291</v>
+      </c>
+      <c r="KW46" t="n">
+        <v>254</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="3">
@@ -43931,8 +44207,14 @@
       <c r="KT47" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="KU47" t="n">
+      <c r="KU47" s="2" t="n">
         <v>72.40000000000001</v>
+      </c>
+      <c r="KV47" s="2" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="KW47" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="3">
@@ -44856,8 +45138,14 @@
       <c r="KT48" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="KU48" t="n">
+      <c r="KU48" s="2" t="n">
         <v>52</v>
+      </c>
+      <c r="KV48" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KW48" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="3">
@@ -45781,8 +46069,14 @@
       <c r="KT49" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KU49" t="n">
+      <c r="KU49" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="KV49" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="KW49" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="3">
@@ -46706,8 +47000,14 @@
       <c r="KT50" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KU50" t="n">
+      <c r="KU50" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="KV50" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="KW50" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="3">
@@ -47631,8 +47931,14 @@
       <c r="KT51" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="KU51" t="n">
+      <c r="KU51" s="2" t="n">
         <v>29</v>
+      </c>
+      <c r="KV51" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KW51" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="3">
@@ -48556,8 +48862,14 @@
       <c r="KT52" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KU52" t="n">
+      <c r="KU52" s="2" t="n">
         <v>37</v>
+      </c>
+      <c r="KV52" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KW52" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="3">
@@ -49481,8 +49793,14 @@
       <c r="KT53" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="KU53" t="n">
+      <c r="KU53" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="KV53" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="KW53" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="3">
@@ -50406,8 +50724,14 @@
       <c r="KT54" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KU54" t="n">
+      <c r="KU54" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="KV54" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="KW54" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="3">
@@ -51331,8 +51655,14 @@
       <c r="KT55" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KU55" t="n">
+      <c r="KU55" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="KV55" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="KW55" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="3">
@@ -52256,8 +52586,14 @@
       <c r="KT56" s="2" t="n">
         <v>61.5</v>
       </c>
-      <c r="KU56" t="n">
+      <c r="KU56" s="2" t="n">
         <v>66.7</v>
+      </c>
+      <c r="KV56" s="2" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="KW56" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="3">
@@ -53181,8 +53517,14 @@
       <c r="KT57" s="2" t="n">
         <v>211</v>
       </c>
-      <c r="KU57" t="n">
+      <c r="KU57" s="2" t="n">
         <v>203</v>
+      </c>
+      <c r="KV57" s="2" t="n">
+        <v>187</v>
+      </c>
+      <c r="KW57" t="n">
+        <v>207</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="3">
@@ -54106,8 +54448,14 @@
       <c r="KT58" s="2" t="n">
         <v>112</v>
       </c>
-      <c r="KU58" t="n">
+      <c r="KU58" s="2" t="n">
         <v>119</v>
+      </c>
+      <c r="KV58" s="2" t="n">
+        <v>144</v>
+      </c>
+      <c r="KW58" t="n">
+        <v>164</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="3">
@@ -55031,8 +55379,14 @@
       <c r="KT59" s="2" t="n">
         <v>323</v>
       </c>
-      <c r="KU59" t="n">
+      <c r="KU59" s="2" t="n">
         <v>322</v>
+      </c>
+      <c r="KV59" s="2" t="n">
+        <v>331</v>
+      </c>
+      <c r="KW59" t="n">
+        <v>371</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="3">
@@ -55956,8 +56310,14 @@
       <c r="KT60" s="2" t="n">
         <v>1.88</v>
       </c>
-      <c r="KU60" t="n">
+      <c r="KU60" s="2" t="n">
         <v>1.71</v>
+      </c>
+      <c r="KV60" s="2" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="KW60" t="n">
+        <v>1.26</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="3">
@@ -56881,8 +57241,14 @@
       <c r="KT61" s="2" t="n">
         <v>94</v>
       </c>
-      <c r="KU61" t="n">
+      <c r="KU61" s="2" t="n">
         <v>69</v>
+      </c>
+      <c r="KV61" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="KW61" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="3">
@@ -57806,8 +58172,14 @@
       <c r="KT62" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="KU62" t="n">
+      <c r="KU62" s="2" t="n">
         <v>54</v>
+      </c>
+      <c r="KV62" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KW62" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="3">
@@ -58731,8 +59103,14 @@
       <c r="KT63" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="KU63" t="n">
+      <c r="KU63" s="2" t="n">
         <v>26</v>
+      </c>
+      <c r="KV63" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="KW63" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="3">
@@ -59656,8 +60034,14 @@
       <c r="KT64" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="KU64" t="n">
+      <c r="KU64" s="2" t="n">
         <v>17</v>
+      </c>
+      <c r="KV64" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="KW64" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="3">
@@ -60581,8 +60965,14 @@
       <c r="KT65" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="KU65" t="n">
+      <c r="KU65" s="2" t="n">
         <v>24</v>
+      </c>
+      <c r="KV65" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="KW65" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="3">
@@ -61506,8 +61896,14 @@
       <c r="KT66" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="KU66" t="n">
+      <c r="KU66" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="KV66" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="KW66" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="3">
@@ -62431,8 +62827,14 @@
       <c r="KT67" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KU67" t="n">
+      <c r="KU67" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="KV67" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KW67" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="3">
@@ -63356,8 +63758,14 @@
       <c r="KT68" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="KU68" t="n">
+      <c r="KU68" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="KV68" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KW68" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="3">
@@ -64281,8 +64689,14 @@
       <c r="KT69" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="KU69" t="n">
+      <c r="KU69" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="KV69" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="KW69" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="3">
@@ -65206,8 +65620,14 @@
       <c r="KT70" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="KU70" t="n">
+      <c r="KU70" s="2" t="n">
         <v>21</v>
+      </c>
+      <c r="KV70" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="KW70" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="3">
@@ -66131,8 +66551,14 @@
       <c r="KT71" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="KU71" t="n">
+      <c r="KU71" s="2" t="n">
         <v>57.1</v>
+      </c>
+      <c r="KV71" s="2" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="KW71" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="3">
@@ -67056,8 +67482,14 @@
       <c r="KT72" s="2" t="n">
         <v>26.92</v>
       </c>
-      <c r="KU72" t="n">
+      <c r="KU72" s="2" t="n">
         <v>26.83</v>
+      </c>
+      <c r="KV72" s="2" t="n">
+        <v>27.58</v>
+      </c>
+      <c r="KW72" t="n">
+        <v>41.22</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="3">
@@ -67981,8 +68413,14 @@
       <c r="KT73" s="2" t="n">
         <v>12.92</v>
       </c>
-      <c r="KU73" t="n">
+      <c r="KU73" s="2" t="n">
         <v>15.33</v>
+      </c>
+      <c r="KV73" s="2" t="n">
+        <v>15.76</v>
+      </c>
+      <c r="KW73" t="n">
+        <v>20.61</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="3">
@@ -68906,8 +69344,14 @@
       <c r="KT74" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KU74" t="n">
+      <c r="KU74" s="2" t="n">
         <v>35</v>
+      </c>
+      <c r="KV74" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="KW74" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="3">
@@ -69831,8 +70275,14 @@
       <c r="KT75" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="KU75" t="n">
+      <c r="KU75" s="2" t="n">
         <v>81</v>
+      </c>
+      <c r="KV75" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="KW75" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="3">
@@ -70756,8 +71206,14 @@
       <c r="KT76" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="KU76" t="n">
+      <c r="KU76" s="2" t="n">
         <v>53</v>
+      </c>
+      <c r="KV76" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KW76" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="3">
@@ -71681,8 +72137,14 @@
       <c r="KT77" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="KU77" t="n">
+      <c r="KU77" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="KV77" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="KW77" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="3">
@@ -72606,8 +73068,14 @@
       <c r="KT78" s="2" t="n">
         <v>2.48</v>
       </c>
-      <c r="KU78" t="n">
+      <c r="KU78" s="2" t="n">
         <v>2.38</v>
+      </c>
+      <c r="KV78" s="2" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="KW78" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="3">
@@ -73531,8 +73999,14 @@
       <c r="KT79" s="2" t="n">
         <v>5.17</v>
       </c>
-      <c r="KU79" t="n">
+      <c r="KU79" s="2" t="n">
         <v>4.17</v>
+      </c>
+      <c r="KV79" s="2" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="KW79" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="3">
@@ -74456,8 +74930,14 @@
       <c r="KT80" s="2" t="n">
         <v>35.5</v>
       </c>
-      <c r="KU80" t="n">
+      <c r="KU80" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="KV80" s="2" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="KW80" t="n">
+        <v>37.8</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="3">
@@ -75381,8 +75861,14 @@
       <c r="KT81" s="2" t="n">
         <v>19.4</v>
       </c>
-      <c r="KU81" t="n">
+      <c r="KU81" s="2" t="n">
         <v>24</v>
+      </c>
+      <c r="KV81" s="2" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="KW81" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="3">
@@ -76306,8 +76792,14 @@
       <c r="KT82" s="2" t="n">
         <v>188</v>
       </c>
-      <c r="KU82" t="n">
+      <c r="KU82" s="2" t="n">
         <v>186.4</v>
+      </c>
+      <c r="KV82" s="2" t="n">
+        <v>188.2</v>
+      </c>
+      <c r="KW82" t="n">
+        <v>188.7</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="3">
@@ -77231,8 +77723,14 @@
       <c r="KT83" s="2" t="n">
         <v>87.09999999999999</v>
       </c>
-      <c r="KU83" t="n">
+      <c r="KU83" s="2" t="n">
         <v>86.3</v>
+      </c>
+      <c r="KV83" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="KW83" t="n">
+        <v>87.3</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="3">
@@ -78156,8 +78654,14 @@
       <c r="KT84" s="2" t="n">
         <v>26.91</v>
       </c>
-      <c r="KU84" t="n">
+      <c r="KU84" s="2" t="n">
         <v>27</v>
+      </c>
+      <c r="KV84" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="KW84" t="n">
+        <v>25.41</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="3">
@@ -79081,8 +79585,14 @@
       <c r="KT85" s="2" t="n">
         <v>133.6</v>
       </c>
-      <c r="KU85" t="n">
+      <c r="KU85" s="2" t="n">
         <v>120.5</v>
+      </c>
+      <c r="KV85" s="2" t="n">
+        <v>64.90000000000001</v>
+      </c>
+      <c r="KW85" t="n">
+        <v>90.40000000000001</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="3">
@@ -80006,8 +80516,14 @@
       <c r="KT86" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="KU86" t="n">
+      <c r="KU86" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="KV86" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KW86" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="3">
@@ -80931,8 +81447,14 @@
       <c r="KT87" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="KU87" t="n">
+      <c r="KU87" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="KV87" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="KW87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="3">
@@ -81856,8 +82378,14 @@
       <c r="KT88" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KU88" t="n">
+      <c r="KU88" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="KV88" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KW88" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="3">
@@ -82781,8 +83309,14 @@
       <c r="KT89" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="KU89" t="n">
+      <c r="KU89" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="KV89" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KW89" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="3">
@@ -83706,8 +84240,14 @@
       <c r="KT90" s="2" t="n">
         <v>133</v>
       </c>
-      <c r="KU90" t="n">
+      <c r="KU90" s="2" t="n">
         <v>142</v>
+      </c>
+      <c r="KV90" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="KW90" t="n">
+        <v>130</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="3">
@@ -84631,8 +85171,14 @@
       <c r="KT91" s="2" t="n">
         <v>183</v>
       </c>
-      <c r="KU91" t="n">
+      <c r="KU91" s="2" t="n">
         <v>169</v>
+      </c>
+      <c r="KV91" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="KW91" t="n">
+        <v>235</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="3">
@@ -85556,8 +86102,14 @@
       <c r="KT92" s="2" t="n">
         <v>229</v>
       </c>
-      <c r="KU92" t="n">
+      <c r="KU92" s="2" t="n">
         <v>213</v>
+      </c>
+      <c r="KV92" s="2" t="n">
+        <v>256</v>
+      </c>
+      <c r="KW92" t="n">
+        <v>283</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="3">
@@ -86481,8 +87033,14 @@
       <c r="KT93" s="2" t="n">
         <v>70.90000000000001</v>
       </c>
-      <c r="KU93" t="n">
+      <c r="KU93" s="2" t="n">
         <v>66.09999999999999</v>
+      </c>
+      <c r="KV93" s="2" t="n">
+        <v>77.3</v>
+      </c>
+      <c r="KW93" t="n">
+        <v>76.3</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="3">
@@ -87406,8 +87964,14 @@
       <c r="KT94" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="KU94" t="n">
+      <c r="KU94" s="2" t="n">
         <v>81</v>
+      </c>
+      <c r="KV94" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="KW94" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="3">
@@ -88331,8 +88895,14 @@
       <c r="KT95" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="KU95" t="n">
+      <c r="KU95" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="KV95" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KW95" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="3">
@@ -89256,8 +89826,14 @@
       <c r="KT96" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="KU96" t="n">
+      <c r="KU96" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="KV96" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="KW96" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="3">
@@ -90181,8 +90757,14 @@
       <c r="KT97" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KU97" t="n">
+      <c r="KU97" s="2" t="n">
         <v>35</v>
+      </c>
+      <c r="KV97" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="KW97" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="3">
@@ -91106,8 +91688,14 @@
       <c r="KT98" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="KU98" t="n">
+      <c r="KU98" s="2" t="n">
         <v>53</v>
+      </c>
+      <c r="KV98" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KW98" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="3">
@@ -92031,8 +92619,14 @@
       <c r="KT99" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="KU99" t="n">
+      <c r="KU99" s="2" t="n">
         <v>46</v>
+      </c>
+      <c r="KV99" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="KW99" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="3">
@@ -92956,8 +93550,14 @@
       <c r="KT100" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KU100" t="n">
+      <c r="KU100" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="KV100" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KW100" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="3">
@@ -93881,8 +94481,14 @@
       <c r="KT101" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KU101" t="n">
+      <c r="KU101" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="KV101" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KW101" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="3">
@@ -94806,8 +95412,14 @@
       <c r="KT102" s="2" t="n">
         <v>58.3</v>
       </c>
-      <c r="KU102" t="n">
+      <c r="KU102" s="2" t="n">
         <v>58.3</v>
+      </c>
+      <c r="KV102" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KW102" t="n">
+        <v>33.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>